<commit_message>
aggiunta parte grafica e collegamentocon il db
</commit_message>
<xml_diff>
--- a/Getsione_magazzino_gantt.xlsx
+++ b/Getsione_magazzino_gantt.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{264B0BF9-45C1-4384-A51C-3708F79C89F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A0D1BD9-11A1-4490-BB66-A38A64B99B9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="57">
   <si>
     <t>Come creare la pianificazione di un progetto in questo foglio di lavoro.
 Immettere il titolo del progetto nella cella B1. 
@@ -267,7 +267,7 @@
     <numFmt numFmtId="168" formatCode="d\ mmm\ yyyy"/>
     <numFmt numFmtId="169" formatCode="d"/>
   </numFmts>
-  <fonts count="34" x14ac:knownFonts="1">
+  <fonts count="35" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -508,6 +508,14 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1038,7 +1046,7 @@
     <xf numFmtId="0" fontId="8" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1260,6 +1268,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="167" fontId="8" fillId="0" borderId="3" xfId="9">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="34" fillId="10" borderId="2" xfId="10" applyFont="1" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1872,8 +1883,8 @@
   <dimension ref="A1:BK31"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
+      <pane ySplit="6" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1923,7 +1934,7 @@
       <c r="C3" s="74"/>
       <c r="D3" s="78">
         <f ca="1">TODAY()</f>
-        <v>45637</v>
+        <v>45813</v>
       </c>
       <c r="E3" s="78"/>
     </row>
@@ -1937,7 +1948,7 @@
       </c>
       <c r="H4" s="75">
         <f ca="1">H5</f>
-        <v>45635</v>
+        <v>45810</v>
       </c>
       <c r="I4" s="76"/>
       <c r="J4" s="76"/>
@@ -1947,7 +1958,7 @@
       <c r="N4" s="77"/>
       <c r="O4" s="75">
         <f ca="1">O5</f>
-        <v>45642</v>
+        <v>45817</v>
       </c>
       <c r="P4" s="76"/>
       <c r="Q4" s="76"/>
@@ -1957,7 +1968,7 @@
       <c r="U4" s="77"/>
       <c r="V4" s="75">
         <f ca="1">V5</f>
-        <v>45649</v>
+        <v>45824</v>
       </c>
       <c r="W4" s="76"/>
       <c r="X4" s="76"/>
@@ -1967,7 +1978,7 @@
       <c r="AB4" s="77"/>
       <c r="AC4" s="75">
         <f ca="1">AC5</f>
-        <v>45656</v>
+        <v>45831</v>
       </c>
       <c r="AD4" s="76"/>
       <c r="AE4" s="76"/>
@@ -1977,7 +1988,7 @@
       <c r="AI4" s="77"/>
       <c r="AJ4" s="75">
         <f ca="1">AJ5</f>
-        <v>45663</v>
+        <v>45838</v>
       </c>
       <c r="AK4" s="76"/>
       <c r="AL4" s="76"/>
@@ -1987,7 +1998,7 @@
       <c r="AP4" s="77"/>
       <c r="AQ4" s="75">
         <f ca="1">AQ5</f>
-        <v>45670</v>
+        <v>45845</v>
       </c>
       <c r="AR4" s="76"/>
       <c r="AS4" s="76"/>
@@ -1997,7 +2008,7 @@
       <c r="AW4" s="77"/>
       <c r="AX4" s="75">
         <f ca="1">AX5</f>
-        <v>45677</v>
+        <v>45852</v>
       </c>
       <c r="AY4" s="76"/>
       <c r="AZ4" s="76"/>
@@ -2007,7 +2018,7 @@
       <c r="BD4" s="77"/>
       <c r="BE4" s="75">
         <f ca="1">BE5</f>
-        <v>45684</v>
+        <v>45859</v>
       </c>
       <c r="BF4" s="76"/>
       <c r="BG4" s="76"/>
@@ -2027,227 +2038,227 @@
       <c r="F5" s="52"/>
       <c r="H5" s="71">
         <f ca="1">Inizio_progetto-WEEKDAY(Inizio_progetto,1)+2+7*(Visualizza_settimana-1)</f>
-        <v>45635</v>
+        <v>45810</v>
       </c>
       <c r="I5" s="72">
         <f ca="1">H5+1</f>
-        <v>45636</v>
+        <v>45811</v>
       </c>
       <c r="J5" s="72">
         <f t="shared" ref="J5:AW5" ca="1" si="0">I5+1</f>
-        <v>45637</v>
+        <v>45812</v>
       </c>
       <c r="K5" s="72">
         <f t="shared" ca="1" si="0"/>
-        <v>45638</v>
+        <v>45813</v>
       </c>
       <c r="L5" s="72">
         <f t="shared" ca="1" si="0"/>
-        <v>45639</v>
+        <v>45814</v>
       </c>
       <c r="M5" s="72">
         <f t="shared" ca="1" si="0"/>
-        <v>45640</v>
+        <v>45815</v>
       </c>
       <c r="N5" s="73">
         <f t="shared" ca="1" si="0"/>
-        <v>45641</v>
+        <v>45816</v>
       </c>
       <c r="O5" s="71">
         <f ca="1">N5+1</f>
-        <v>45642</v>
+        <v>45817</v>
       </c>
       <c r="P5" s="72">
         <f ca="1">O5+1</f>
-        <v>45643</v>
+        <v>45818</v>
       </c>
       <c r="Q5" s="72">
         <f t="shared" ca="1" si="0"/>
-        <v>45644</v>
+        <v>45819</v>
       </c>
       <c r="R5" s="72">
         <f t="shared" ca="1" si="0"/>
-        <v>45645</v>
+        <v>45820</v>
       </c>
       <c r="S5" s="72">
         <f t="shared" ca="1" si="0"/>
-        <v>45646</v>
+        <v>45821</v>
       </c>
       <c r="T5" s="72">
         <f t="shared" ca="1" si="0"/>
-        <v>45647</v>
+        <v>45822</v>
       </c>
       <c r="U5" s="73">
         <f t="shared" ca="1" si="0"/>
-        <v>45648</v>
+        <v>45823</v>
       </c>
       <c r="V5" s="71">
         <f ca="1">U5+1</f>
-        <v>45649</v>
+        <v>45824</v>
       </c>
       <c r="W5" s="72">
         <f ca="1">V5+1</f>
-        <v>45650</v>
+        <v>45825</v>
       </c>
       <c r="X5" s="72">
         <f t="shared" ca="1" si="0"/>
-        <v>45651</v>
+        <v>45826</v>
       </c>
       <c r="Y5" s="72">
         <f t="shared" ca="1" si="0"/>
-        <v>45652</v>
+        <v>45827</v>
       </c>
       <c r="Z5" s="72">
         <f t="shared" ca="1" si="0"/>
-        <v>45653</v>
+        <v>45828</v>
       </c>
       <c r="AA5" s="72">
         <f t="shared" ca="1" si="0"/>
-        <v>45654</v>
+        <v>45829</v>
       </c>
       <c r="AB5" s="73">
         <f t="shared" ca="1" si="0"/>
-        <v>45655</v>
+        <v>45830</v>
       </c>
       <c r="AC5" s="71">
         <f ca="1">AB5+1</f>
-        <v>45656</v>
+        <v>45831</v>
       </c>
       <c r="AD5" s="72">
         <f ca="1">AC5+1</f>
-        <v>45657</v>
+        <v>45832</v>
       </c>
       <c r="AE5" s="72">
         <f t="shared" ca="1" si="0"/>
-        <v>45658</v>
+        <v>45833</v>
       </c>
       <c r="AF5" s="72">
         <f t="shared" ca="1" si="0"/>
-        <v>45659</v>
+        <v>45834</v>
       </c>
       <c r="AG5" s="72">
         <f t="shared" ca="1" si="0"/>
-        <v>45660</v>
+        <v>45835</v>
       </c>
       <c r="AH5" s="72">
         <f t="shared" ca="1" si="0"/>
-        <v>45661</v>
+        <v>45836</v>
       </c>
       <c r="AI5" s="73">
         <f t="shared" ca="1" si="0"/>
-        <v>45662</v>
+        <v>45837</v>
       </c>
       <c r="AJ5" s="71">
         <f ca="1">AI5+1</f>
-        <v>45663</v>
+        <v>45838</v>
       </c>
       <c r="AK5" s="72">
         <f ca="1">AJ5+1</f>
-        <v>45664</v>
+        <v>45839</v>
       </c>
       <c r="AL5" s="72">
         <f t="shared" ca="1" si="0"/>
-        <v>45665</v>
+        <v>45840</v>
       </c>
       <c r="AM5" s="72">
         <f t="shared" ca="1" si="0"/>
-        <v>45666</v>
+        <v>45841</v>
       </c>
       <c r="AN5" s="72">
         <f t="shared" ca="1" si="0"/>
-        <v>45667</v>
+        <v>45842</v>
       </c>
       <c r="AO5" s="72">
         <f t="shared" ca="1" si="0"/>
-        <v>45668</v>
+        <v>45843</v>
       </c>
       <c r="AP5" s="73">
         <f t="shared" ca="1" si="0"/>
-        <v>45669</v>
+        <v>45844</v>
       </c>
       <c r="AQ5" s="71">
         <f ca="1">AP5+1</f>
-        <v>45670</v>
+        <v>45845</v>
       </c>
       <c r="AR5" s="72">
         <f ca="1">AQ5+1</f>
-        <v>45671</v>
+        <v>45846</v>
       </c>
       <c r="AS5" s="72">
         <f t="shared" ca="1" si="0"/>
-        <v>45672</v>
+        <v>45847</v>
       </c>
       <c r="AT5" s="72">
         <f t="shared" ca="1" si="0"/>
-        <v>45673</v>
+        <v>45848</v>
       </c>
       <c r="AU5" s="72">
         <f t="shared" ca="1" si="0"/>
-        <v>45674</v>
+        <v>45849</v>
       </c>
       <c r="AV5" s="72">
         <f t="shared" ca="1" si="0"/>
-        <v>45675</v>
+        <v>45850</v>
       </c>
       <c r="AW5" s="73">
         <f t="shared" ca="1" si="0"/>
-        <v>45676</v>
+        <v>45851</v>
       </c>
       <c r="AX5" s="71">
         <f ca="1">AW5+1</f>
-        <v>45677</v>
+        <v>45852</v>
       </c>
       <c r="AY5" s="72">
         <f ca="1">AX5+1</f>
-        <v>45678</v>
+        <v>45853</v>
       </c>
       <c r="AZ5" s="72">
         <f t="shared" ref="AZ5:BD5" ca="1" si="1">AY5+1</f>
-        <v>45679</v>
+        <v>45854</v>
       </c>
       <c r="BA5" s="72">
         <f t="shared" ca="1" si="1"/>
-        <v>45680</v>
+        <v>45855</v>
       </c>
       <c r="BB5" s="72">
         <f t="shared" ca="1" si="1"/>
-        <v>45681</v>
+        <v>45856</v>
       </c>
       <c r="BC5" s="72">
         <f t="shared" ca="1" si="1"/>
-        <v>45682</v>
+        <v>45857</v>
       </c>
       <c r="BD5" s="73">
         <f t="shared" ca="1" si="1"/>
-        <v>45683</v>
+        <v>45858</v>
       </c>
       <c r="BE5" s="71">
         <f ca="1">BD5+1</f>
-        <v>45684</v>
+        <v>45859</v>
       </c>
       <c r="BF5" s="72">
         <f ca="1">BE5+1</f>
-        <v>45685</v>
+        <v>45860</v>
       </c>
       <c r="BG5" s="72">
         <f t="shared" ref="BG5:BK5" ca="1" si="2">BF5+1</f>
-        <v>45686</v>
+        <v>45861</v>
       </c>
       <c r="BH5" s="72">
         <f t="shared" ca="1" si="2"/>
-        <v>45687</v>
+        <v>45862</v>
       </c>
       <c r="BI5" s="72">
         <f t="shared" ca="1" si="2"/>
-        <v>45688</v>
+        <v>45863</v>
       </c>
       <c r="BJ5" s="72">
         <f t="shared" ca="1" si="2"/>
-        <v>45689</v>
+        <v>45864</v>
       </c>
       <c r="BK5" s="73">
         <f t="shared" ca="1" si="2"/>
-        <v>45690</v>
+        <v>45865</v>
       </c>
     </row>
     <row r="6" spans="1:63" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -2645,11 +2656,11 @@
       </c>
       <c r="D9" s="58">
         <f ca="1">Inizio_progetto</f>
-        <v>45637</v>
+        <v>45813</v>
       </c>
       <c r="E9" s="58">
         <f ca="1">D9+3</f>
-        <v>45640</v>
+        <v>45816</v>
       </c>
       <c r="F9" s="11"/>
       <c r="G9" s="11">
@@ -2725,11 +2736,11 @@
       </c>
       <c r="D10" s="58">
         <f ca="1">E9</f>
-        <v>45640</v>
+        <v>45816</v>
       </c>
       <c r="E10" s="58">
         <f ca="1">D10+2</f>
-        <v>45642</v>
+        <v>45818</v>
       </c>
       <c r="F10" s="11"/>
       <c r="G10" s="11">
@@ -2803,11 +2814,11 @@
       </c>
       <c r="D11" s="58">
         <f ca="1">E10</f>
-        <v>45642</v>
+        <v>45818</v>
       </c>
       <c r="E11" s="58">
         <f ca="1">D11+4</f>
-        <v>45646</v>
+        <v>45822</v>
       </c>
       <c r="F11" s="11"/>
       <c r="G11" s="11">
@@ -2881,11 +2892,11 @@
       </c>
       <c r="D12" s="58">
         <f ca="1">E11</f>
-        <v>45646</v>
+        <v>45822</v>
       </c>
       <c r="E12" s="58">
         <f ca="1">D12+5</f>
-        <v>45651</v>
+        <v>45827</v>
       </c>
       <c r="F12" s="11"/>
       <c r="G12" s="11">
@@ -3031,11 +3042,11 @@
       </c>
       <c r="D14" s="61">
         <f ca="1">D12+1</f>
-        <v>45647</v>
+        <v>45823</v>
       </c>
       <c r="E14" s="61">
         <f ca="1">D14+4</f>
-        <v>45651</v>
+        <v>45827</v>
       </c>
       <c r="F14" s="11"/>
       <c r="G14" s="11">
@@ -3109,11 +3120,11 @@
       </c>
       <c r="D15" s="61">
         <f ca="1">D14+2</f>
-        <v>45649</v>
+        <v>45825</v>
       </c>
       <c r="E15" s="61">
         <f ca="1">D15+5</f>
-        <v>45654</v>
+        <v>45830</v>
       </c>
       <c r="F15" s="11"/>
       <c r="G15" s="11">
@@ -3187,11 +3198,11 @@
       </c>
       <c r="D16" s="61">
         <f ca="1">E15</f>
-        <v>45654</v>
+        <v>45830</v>
       </c>
       <c r="E16" s="61">
         <f ca="1">D16+3</f>
-        <v>45657</v>
+        <v>45833</v>
       </c>
       <c r="F16" s="11"/>
       <c r="G16" s="11">
@@ -3265,11 +3276,11 @@
       </c>
       <c r="D17" s="61">
         <f ca="1">D16</f>
-        <v>45654</v>
+        <v>45830</v>
       </c>
       <c r="E17" s="61">
         <f ca="1">D17+2</f>
-        <v>45656</v>
+        <v>45832</v>
       </c>
       <c r="F17" s="11"/>
       <c r="G17" s="11">
@@ -3343,11 +3354,11 @@
       </c>
       <c r="D18" s="61">
         <f ca="1">D17</f>
-        <v>45654</v>
+        <v>45830</v>
       </c>
       <c r="E18" s="61">
         <f ca="1">D18+3</f>
-        <v>45657</v>
+        <v>45833</v>
       </c>
       <c r="F18" s="11"/>
       <c r="G18" s="11">
@@ -3489,15 +3500,15 @@
         <v>51</v>
       </c>
       <c r="C20" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D20" s="64">
         <f ca="1">D9+15</f>
-        <v>45652</v>
+        <v>45828</v>
       </c>
       <c r="E20" s="64">
         <f ca="1">D20+5</f>
-        <v>45657</v>
+        <v>45833</v>
       </c>
       <c r="F20" s="11"/>
       <c r="G20" s="11">
@@ -3567,15 +3578,15 @@
         <v>52</v>
       </c>
       <c r="C21" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21" s="64">
         <f ca="1">E20+1</f>
-        <v>45658</v>
+        <v>45834</v>
       </c>
       <c r="E21" s="64">
         <f ca="1">D21+4</f>
-        <v>45662</v>
+        <v>45838</v>
       </c>
       <c r="F21" s="11"/>
       <c r="G21" s="11">
@@ -3645,15 +3656,15 @@
         <v>53</v>
       </c>
       <c r="C22" s="20">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="D22" s="64">
         <f ca="1">D21+5</f>
-        <v>45663</v>
+        <v>45839</v>
       </c>
       <c r="E22" s="64">
         <f ca="1">D22+5</f>
-        <v>45668</v>
+        <v>45844</v>
       </c>
       <c r="F22" s="11"/>
       <c r="G22" s="11">
@@ -3795,18 +3806,20 @@
         <v>54</v>
       </c>
       <c r="C24" s="23">
-        <v>0</v>
-      </c>
-      <c r="D24" s="67" t="s">
-        <v>27</v>
-      </c>
-      <c r="E24" s="67" t="s">
-        <v>27</v>
+        <v>0.4</v>
+      </c>
+      <c r="D24" s="67">
+        <f ca="1">E22-1</f>
+        <v>45843</v>
+      </c>
+      <c r="E24" s="67">
+        <f ca="1">D24+6</f>
+        <v>45849</v>
       </c>
       <c r="F24" s="11"/>
-      <c r="G24" s="11" t="e">
-        <f t="shared" si="5"/>
-        <v>#VALUE!</v>
+      <c r="G24" s="11">
+        <f t="shared" ca="1" si="5"/>
+        <v>7</v>
       </c>
       <c r="H24" s="27"/>
       <c r="I24" s="27"/>
@@ -3871,18 +3884,20 @@
         <v>55</v>
       </c>
       <c r="C25" s="23">
-        <v>0</v>
-      </c>
-      <c r="D25" s="67" t="s">
-        <v>27</v>
-      </c>
-      <c r="E25" s="67" t="s">
-        <v>27</v>
+        <v>0.3</v>
+      </c>
+      <c r="D25" s="67">
+        <f ca="1">E24+1</f>
+        <v>45850</v>
+      </c>
+      <c r="E25" s="67">
+        <f ca="1">D25+4</f>
+        <v>45854</v>
       </c>
       <c r="F25" s="11"/>
-      <c r="G25" s="11" t="e">
-        <f t="shared" si="5"/>
-        <v>#VALUE!</v>
+      <c r="G25" s="11">
+        <f t="shared" ca="1" si="5"/>
+        <v>5</v>
       </c>
       <c r="H25" s="27"/>
       <c r="I25" s="27"/>
@@ -3952,7 +3967,7 @@
       <c r="D26" s="67" t="s">
         <v>27</v>
       </c>
-      <c r="E26" s="67" t="s">
+      <c r="E26" s="79" t="s">
         <v>27</v>
       </c>
       <c r="F26" s="11"/>
@@ -4432,23 +4447,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4740,22 +4744,29 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5144944C-1F1D-4162-962A-96F3FC8455D8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FE8ED85-58B3-4608-8E91-0433556D50CE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4782,9 +4793,13 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FE8ED85-58B3-4608-8E91-0433556D50CE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5144944C-1F1D-4162-962A-96F3FC8455D8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>